<commit_message>
Version with both global and distrubuted popped and unique sets
</commit_message>
<xml_diff>
--- a/GSS.xlsx
+++ b/GSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janwillem/Library/Mobile Documents/com~apple~CloudDocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEB1FC7-8660-2A46-9C7C-FB4F20DD1A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545AEEC3-5DE3-5C44-AFD6-6DCC3876C51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{AA8DE287-894B-054D-B4F4-0AAA604E9440}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{AA8DE287-894B-054D-B4F4-0AAA604E9440}"/>
   </bookViews>
   <sheets>
     <sheet name="S = x x x" sheetId="9" r:id="rId1"/>
@@ -1072,9 +1072,6 @@
     <t>A.#.0 B.#.0 E.#.0 B.D0.0 E.D0.0</t>
   </si>
   <si>
-    <t>add D,D0,0</t>
-  </si>
-  <si>
     <t>A.#.0 B.#.0 E.#.0 B.D0.0 E.D0.0 D.D0.0</t>
   </si>
   <si>
@@ -1082,6 +1079,9 @@
   </si>
   <si>
     <t>get D.D0.0</t>
+  </si>
+  <si>
+    <t>add D.D0.0</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1592,9 +1592,6 @@
     <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1718,7 +1715,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4865,7 +4862,7 @@
       <c r="C3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="97" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="38"/>
@@ -4943,13 +4940,13 @@
       <c r="B5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="97" t="s">
         <v>33</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="97" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="38"/>
@@ -5024,7 +5021,7 @@
       <c r="B7" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="97" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="38"/>
@@ -5206,11 +5203,11 @@
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
-      <c r="F12" s="99" t="s">
+      <c r="F12" s="98" t="s">
         <v>83</v>
       </c>
       <c r="G12" s="39"/>
-      <c r="H12" s="99" t="s">
+      <c r="H12" s="98" t="s">
         <v>81</v>
       </c>
       <c r="I12" s="39"/>
@@ -5218,7 +5215,7 @@
         <v>86</v>
       </c>
       <c r="K12" s="39"/>
-      <c r="L12" s="99" t="s">
+      <c r="L12" s="98" t="s">
         <v>111</v>
       </c>
       <c r="M12" s="39"/>
@@ -5246,13 +5243,13 @@
       <c r="E13" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="99" t="s">
+      <c r="F13" s="98" t="s">
         <v>70</v>
       </c>
       <c r="G13" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="99" t="s">
+      <c r="H13" s="98" t="s">
         <v>79</v>
       </c>
       <c r="I13" s="39" t="s">
@@ -5264,7 +5261,7 @@
       <c r="K13" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="99" t="s">
+      <c r="L13" s="98" t="s">
         <v>110</v>
       </c>
       <c r="M13" s="15" t="s">
@@ -5295,19 +5292,19 @@
       <c r="D14" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="100" t="s">
+      <c r="E14" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="F14" s="101" t="s">
+      <c r="F14" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="102" t="s">
+      <c r="G14" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="103" t="s">
+      <c r="H14" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="104" t="s">
+      <c r="I14" s="103" t="s">
         <v>82</v>
       </c>
       <c r="J14" s="45" t="s">
@@ -5316,7 +5313,7 @@
       <c r="K14" s="83" t="s">
         <v>82</v>
       </c>
-      <c r="L14" s="105" t="s">
+      <c r="L14" s="104" t="s">
         <v>82</v>
       </c>
       <c r="M14" s="15" t="s">
@@ -5347,19 +5344,19 @@
       <c r="D15" s="39">
         <v>0</v>
       </c>
-      <c r="E15" s="100">
+      <c r="E15" s="99">
         <v>0</v>
       </c>
-      <c r="F15" s="101">
+      <c r="F15" s="100">
         <v>0</v>
       </c>
-      <c r="G15" s="102">
+      <c r="G15" s="101">
         <v>1</v>
       </c>
-      <c r="H15" s="103">
+      <c r="H15" s="102">
         <v>1</v>
       </c>
-      <c r="I15" s="104">
+      <c r="I15" s="103">
         <v>2</v>
       </c>
       <c r="J15" s="45">
@@ -5368,7 +5365,7 @@
       <c r="K15" s="83">
         <v>3</v>
       </c>
-      <c r="L15" s="105">
+      <c r="L15" s="104">
         <v>3</v>
       </c>
       <c r="M15" s="15">
@@ -5396,13 +5393,13 @@
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
-      <c r="F16" s="99"/>
+      <c r="F16" s="98"/>
       <c r="G16" s="39"/>
-      <c r="H16" s="99"/>
+      <c r="H16" s="98"/>
       <c r="I16" s="39"/>
       <c r="J16" s="44"/>
       <c r="K16" s="39"/>
-      <c r="L16" s="99"/>
+      <c r="L16" s="98"/>
       <c r="M16" s="39"/>
       <c r="S16" s="39"/>
       <c r="T16" s="39"/>
@@ -5426,13 +5423,13 @@
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
-      <c r="F17" s="99"/>
+      <c r="F17" s="98"/>
       <c r="G17" s="39"/>
-      <c r="H17" s="99"/>
+      <c r="H17" s="98"/>
       <c r="I17" s="39"/>
       <c r="J17" s="44"/>
       <c r="K17" s="39"/>
-      <c r="L17" s="99"/>
+      <c r="L17" s="98"/>
       <c r="M17" s="39"/>
       <c r="S17" s="39"/>
       <c r="T17" s="39"/>
@@ -5458,17 +5455,17 @@
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
       <c r="E18" s="39"/>
-      <c r="F18" s="101" t="s">
+      <c r="F18" s="100" t="s">
         <v>82</v>
       </c>
       <c r="G18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="99"/>
+      <c r="H18" s="98"/>
       <c r="I18" s="39"/>
       <c r="J18" s="44"/>
       <c r="K18" s="39"/>
-      <c r="L18" s="99"/>
+      <c r="L18" s="98"/>
       <c r="M18" s="39"/>
       <c r="S18" s="39"/>
       <c r="T18" s="39"/>
@@ -5494,17 +5491,17 @@
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
       <c r="E19" s="39"/>
-      <c r="F19" s="101">
+      <c r="F19" s="100">
         <v>0</v>
       </c>
       <c r="G19" s="15">
         <v>1</v>
       </c>
-      <c r="H19" s="99"/>
+      <c r="H19" s="98"/>
       <c r="I19" s="39"/>
       <c r="J19" s="44"/>
       <c r="K19" s="39"/>
-      <c r="L19" s="99"/>
+      <c r="L19" s="98"/>
       <c r="M19" s="39"/>
       <c r="S19" s="39"/>
       <c r="T19" s="39"/>
@@ -5530,11 +5527,11 @@
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
-      <c r="H20" s="99"/>
+      <c r="H20" s="98"/>
       <c r="I20" s="39"/>
       <c r="J20" s="44"/>
       <c r="K20" s="39"/>
-      <c r="L20" s="99"/>
+      <c r="L20" s="98"/>
       <c r="M20" s="39"/>
       <c r="S20" s="39"/>
       <c r="T20" s="39"/>
@@ -5560,11 +5557,11 @@
       <c r="E21" s="39"/>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
-      <c r="H21" s="99"/>
+      <c r="H21" s="98"/>
       <c r="I21" s="39"/>
       <c r="J21" s="44"/>
       <c r="K21" s="39"/>
-      <c r="L21" s="99"/>
+      <c r="L21" s="98"/>
       <c r="M21" s="39"/>
       <c r="S21" s="39"/>
       <c r="T21" s="39"/>
@@ -5592,7 +5589,7 @@
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
-      <c r="H22" s="103" t="s">
+      <c r="H22" s="102" t="s">
         <v>82</v>
       </c>
       <c r="I22" s="15" t="s">
@@ -5600,7 +5597,7 @@
       </c>
       <c r="J22" s="44"/>
       <c r="K22" s="39"/>
-      <c r="L22" s="99"/>
+      <c r="L22" s="98"/>
       <c r="M22" s="39"/>
       <c r="S22" s="39"/>
       <c r="T22" s="39"/>
@@ -5628,7 +5625,7 @@
       <c r="E23" s="39"/>
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
-      <c r="H23" s="103">
+      <c r="H23" s="102">
         <v>1</v>
       </c>
       <c r="I23" s="15">
@@ -5636,7 +5633,7 @@
       </c>
       <c r="J23" s="44"/>
       <c r="K23" s="39"/>
-      <c r="L23" s="99"/>
+      <c r="L23" s="98"/>
       <c r="M23" s="39"/>
       <c r="S23" s="39"/>
       <c r="T23" s="39"/>
@@ -5666,7 +5663,7 @@
       <c r="I24" s="39"/>
       <c r="J24" s="44"/>
       <c r="K24" s="39"/>
-      <c r="L24" s="99"/>
+      <c r="L24" s="98"/>
       <c r="M24" s="39"/>
       <c r="S24" s="39"/>
       <c r="T24" s="39"/>
@@ -5696,7 +5693,7 @@
       <c r="I25" s="39"/>
       <c r="J25" s="44"/>
       <c r="K25" s="39"/>
-      <c r="L25" s="99"/>
+      <c r="L25" s="98"/>
       <c r="M25" s="39"/>
       <c r="S25" s="39"/>
       <c r="T25" s="39"/>
@@ -5726,7 +5723,7 @@
       <c r="I26" s="39"/>
       <c r="J26" s="44"/>
       <c r="K26" s="39"/>
-      <c r="L26" s="99"/>
+      <c r="L26" s="98"/>
       <c r="M26" s="39"/>
       <c r="S26" s="39"/>
       <c r="T26" s="39"/>
@@ -5762,7 +5759,7 @@
       <c r="K27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="L27" s="99"/>
+      <c r="L27" s="98"/>
       <c r="M27" s="39"/>
       <c r="S27" s="39"/>
       <c r="T27" s="39"/>
@@ -5798,7 +5795,7 @@
       <c r="K28" s="14">
         <v>3</v>
       </c>
-      <c r="L28" s="99"/>
+      <c r="L28" s="98"/>
       <c r="M28" s="39"/>
       <c r="S28" s="39"/>
       <c r="T28" s="39"/>
@@ -5828,7 +5825,7 @@
       <c r="I29" s="39"/>
       <c r="J29" s="39"/>
       <c r="K29" s="39"/>
-      <c r="L29" s="99"/>
+      <c r="L29" s="98"/>
       <c r="M29" s="39"/>
       <c r="S29" s="39"/>
       <c r="T29" s="39"/>
@@ -5858,7 +5855,7 @@
       <c r="I30" s="39"/>
       <c r="J30" s="39"/>
       <c r="K30" s="39"/>
-      <c r="L30" s="99"/>
+      <c r="L30" s="98"/>
       <c r="M30" s="39"/>
       <c r="S30" s="39"/>
       <c r="T30" s="39"/>
@@ -5890,7 +5887,7 @@
       <c r="I31" s="39"/>
       <c r="J31" s="39"/>
       <c r="K31" s="39"/>
-      <c r="L31" s="105" t="s">
+      <c r="L31" s="104" t="s">
         <v>82</v>
       </c>
       <c r="M31" s="15" t="s">
@@ -5926,7 +5923,7 @@
       <c r="I32" s="39"/>
       <c r="J32" s="39"/>
       <c r="K32" s="39"/>
-      <c r="L32" s="105">
+      <c r="L32" s="104">
         <v>3</v>
       </c>
       <c r="M32" s="15">
@@ -6183,7 +6180,7 @@
       <c r="C3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="97" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="38"/>
@@ -6211,7 +6208,7 @@
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="F4" s="38"/>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="96" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="39" t="s">
@@ -6238,19 +6235,19 @@
       <c r="A5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="97" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="97" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="97" t="s">
         <v>33</v>
       </c>
       <c r="H5" s="40" t="s">
@@ -6311,13 +6308,13 @@
       <c r="A7" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="97" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="98" t="s">
+      <c r="F7" s="97" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="40" t="s">
@@ -6490,7 +6487,7 @@
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
-      <c r="L13" s="99" t="s">
+      <c r="L13" s="98" t="s">
         <v>41</v>
       </c>
       <c r="M13" s="38"/>
@@ -6517,7 +6514,7 @@
       <c r="I14" s="39"/>
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
-      <c r="L14" s="99" t="s">
+      <c r="L14" s="98" t="s">
         <v>7</v>
       </c>
       <c r="M14" s="15" t="s">
@@ -6546,7 +6543,7 @@
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
-      <c r="L15" s="101">
+      <c r="L15" s="100">
         <v>3</v>
       </c>
       <c r="M15" s="15">
@@ -6612,7 +6609,7 @@
       <c r="K17" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="106" t="s">
+      <c r="L17" s="105" t="s">
         <v>21</v>
       </c>
       <c r="M17" s="16"/>
@@ -6645,7 +6642,7 @@
       <c r="K18" s="50">
         <v>3</v>
       </c>
-      <c r="L18" s="107">
+      <c r="L18" s="106">
         <v>3</v>
       </c>
       <c r="M18" s="14" t="s">
@@ -6704,7 +6701,7 @@
       <c r="I20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J20" s="108" t="s">
+      <c r="J20" s="107" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="16"/>
@@ -6730,13 +6727,13 @@
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
-      <c r="H21" s="109">
+      <c r="H21" s="108">
         <v>1</v>
       </c>
       <c r="I21" s="20">
         <v>2</v>
       </c>
-      <c r="J21" s="110">
+      <c r="J21" s="109">
         <v>2</v>
       </c>
       <c r="K21" s="15" t="s">
@@ -6791,7 +6788,7 @@
       <c r="E23" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="111" t="s">
+      <c r="F23" s="110" t="s">
         <v>5</v>
       </c>
       <c r="G23" s="16"/>
@@ -6827,13 +6824,13 @@
       <c r="E24" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="111" t="s">
+      <c r="F24" s="110" t="s">
         <v>7</v>
       </c>
       <c r="G24" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="108" t="s">
+      <c r="H24" s="107" t="s">
         <v>21</v>
       </c>
       <c r="I24" s="16"/>
@@ -6867,13 +6864,13 @@
       <c r="E25" s="83">
         <v>0</v>
       </c>
-      <c r="F25" s="111">
+      <c r="F25" s="110">
         <v>0</v>
       </c>
       <c r="G25" s="67">
         <v>1</v>
       </c>
-      <c r="H25" s="112">
+      <c r="H25" s="111">
         <v>1</v>
       </c>
       <c r="I25" s="15" t="s">
@@ -6931,19 +6928,19 @@
       <c r="C27" s="39"/>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="99" t="s">
+      <c r="F27" s="98" t="s">
         <v>8</v>
       </c>
       <c r="G27" s="39"/>
-      <c r="H27" s="99" t="s">
+      <c r="H27" s="98" t="s">
         <v>8</v>
       </c>
       <c r="I27" s="39"/>
-      <c r="J27" s="99" t="s">
+      <c r="J27" s="98" t="s">
         <v>8</v>
       </c>
       <c r="K27" s="39"/>
-      <c r="L27" s="99" t="s">
+      <c r="L27" s="98" t="s">
         <v>8</v>
       </c>
       <c r="M27" s="39"/>
@@ -6967,13 +6964,13 @@
       <c r="C28" s="39"/>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="99" t="s">
+      <c r="F28" s="98" t="s">
         <v>3</v>
       </c>
       <c r="G28" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="99" t="s">
+      <c r="H28" s="98" t="s">
         <v>3</v>
       </c>
       <c r="I28" s="39" t="s">
@@ -6985,7 +6982,7 @@
       <c r="K28" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="L28" s="99" t="s">
+      <c r="L28" s="98" t="s">
         <v>3</v>
       </c>
       <c r="M28" s="15" t="s">
@@ -7010,25 +7007,25 @@
       <c r="C29" s="39"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="105" t="s">
+      <c r="F29" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="102" t="s">
+      <c r="G29" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="103" t="s">
+      <c r="H29" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="I29" s="104" t="s">
+      <c r="I29" s="103" t="s">
         <v>5</v>
       </c>
       <c r="J29" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="100" t="s">
+      <c r="K29" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="101" t="s">
+      <c r="L29" s="100" t="s">
         <v>5</v>
       </c>
       <c r="M29" s="15" t="s">
@@ -7056,25 +7053,25 @@
       <c r="C30" s="39"/>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="105" t="s">
+      <c r="F30" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="102" t="s">
+      <c r="G30" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="103" t="s">
+      <c r="H30" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="104" t="s">
+      <c r="I30" s="103" t="s">
         <v>7</v>
       </c>
       <c r="J30" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="K30" s="100" t="s">
+      <c r="K30" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="L30" s="101" t="s">
+      <c r="L30" s="100" t="s">
         <v>7</v>
       </c>
       <c r="M30" s="15" t="s">
@@ -7102,25 +7099,25 @@
       <c r="C31" s="39"/>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="105">
+      <c r="F31" s="104">
         <v>0</v>
       </c>
-      <c r="G31" s="102">
+      <c r="G31" s="101">
         <v>1</v>
       </c>
-      <c r="H31" s="103">
+      <c r="H31" s="102">
         <v>1</v>
       </c>
-      <c r="I31" s="104">
+      <c r="I31" s="103">
         <v>2</v>
       </c>
       <c r="J31" s="45">
         <v>2</v>
       </c>
-      <c r="K31" s="100">
+      <c r="K31" s="99">
         <v>3</v>
       </c>
-      <c r="L31" s="101">
+      <c r="L31" s="100">
         <v>3</v>
       </c>
       <c r="M31" s="15">
@@ -7179,7 +7176,7 @@
       <c r="H33" s="55"/>
       <c r="J33" s="55"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="101" t="s">
+      <c r="L33" s="100" t="s">
         <v>5</v>
       </c>
       <c r="M33" s="16"/>
@@ -7209,7 +7206,7 @@
       <c r="H34" s="55"/>
       <c r="J34" s="55"/>
       <c r="K34" s="16"/>
-      <c r="L34" s="101" t="s">
+      <c r="L34" s="100" t="s">
         <v>7</v>
       </c>
       <c r="M34" s="15" t="s">
@@ -7241,7 +7238,7 @@
       <c r="H35" s="55"/>
       <c r="J35" s="55"/>
       <c r="K35" s="16"/>
-      <c r="L35" s="101">
+      <c r="L35" s="100">
         <v>3</v>
       </c>
       <c r="M35" s="15">
@@ -7298,7 +7295,7 @@
       <c r="G37" s="16"/>
       <c r="H37" s="55"/>
       <c r="I37" s="16"/>
-      <c r="J37" s="113" t="s">
+      <c r="J37" s="112" t="s">
         <v>5</v>
       </c>
       <c r="K37" s="16"/>
@@ -7330,13 +7327,13 @@
       <c r="G38" s="16"/>
       <c r="H38" s="55"/>
       <c r="I38" s="16"/>
-      <c r="J38" s="113" t="s">
+      <c r="J38" s="112" t="s">
         <v>7</v>
       </c>
       <c r="K38" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L38" s="106" t="s">
+      <c r="L38" s="105" t="s">
         <v>21</v>
       </c>
       <c r="M38" s="16"/>
@@ -7364,13 +7361,13 @@
       <c r="G39" s="16"/>
       <c r="H39" s="55"/>
       <c r="I39" s="16"/>
-      <c r="J39" s="113">
+      <c r="J39" s="112">
         <v>2</v>
       </c>
       <c r="K39" s="83">
         <v>3</v>
       </c>
-      <c r="L39" s="114">
+      <c r="L39" s="113">
         <v>3</v>
       </c>
       <c r="M39" s="14" t="s">
@@ -7394,7 +7391,7 @@
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
-      <c r="H41" s="103" t="s">
+      <c r="H41" s="102" t="s">
         <v>5</v>
       </c>
       <c r="I41" s="16"/>
@@ -7413,13 +7410,13 @@
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="103" t="s">
+      <c r="H42" s="102" t="s">
         <v>7</v>
       </c>
       <c r="I42" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J42" s="108" t="s">
+      <c r="J42" s="107" t="s">
         <v>21</v>
       </c>
       <c r="K42" s="16"/>
@@ -7438,7 +7435,7 @@
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
-      <c r="H43" s="103">
+      <c r="H43" s="102">
         <v>1</v>
       </c>
       <c r="I43" s="50">
@@ -7450,7 +7447,7 @@
       <c r="K43" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="L43" s="111">
+      <c r="L43" s="110">
         <v>3</v>
       </c>
       <c r="M43" s="15">
@@ -7502,7 +7499,7 @@
       <c r="K46" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="L46" s="106" t="s">
+      <c r="L46" s="105" t="s">
         <v>21</v>
       </c>
       <c r="M46" s="16"/>
@@ -7523,7 +7520,7 @@
       <c r="K47" s="20">
         <v>3</v>
       </c>
-      <c r="L47" s="115">
+      <c r="L47" s="114">
         <v>3</v>
       </c>
       <c r="M47" s="14" t="s">
@@ -9019,7 +9016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80C9975-078B-E140-84CA-F25E0862AB0D}">
   <dimension ref="A1:AR114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
@@ -9079,18 +9076,18 @@
       <c r="AF1" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="AG1" s="96"/>
+      <c r="AG1" s="95"/>
       <c r="AH1" s="76"/>
-      <c r="AI1" s="96"/>
-      <c r="AJ1" s="96"/>
-      <c r="AK1" s="96"/>
-      <c r="AL1" s="96"/>
-      <c r="AM1" s="96"/>
-      <c r="AN1" s="96"/>
-      <c r="AO1" s="96"/>
-      <c r="AP1" s="96"/>
-      <c r="AQ1" s="96"/>
-      <c r="AR1" s="96"/>
+      <c r="AI1" s="95"/>
+      <c r="AJ1" s="95"/>
+      <c r="AK1" s="95"/>
+      <c r="AL1" s="95"/>
+      <c r="AM1" s="95"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="95"/>
+      <c r="AP1" s="95"/>
+      <c r="AQ1" s="95"/>
+      <c r="AR1" s="95"/>
     </row>
     <row r="2" spans="1:44">
       <c r="A2" s="38"/>
@@ -23461,8 +23458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FAC3B8C-48C5-224C-B47A-1E674A612C9A}">
   <dimension ref="A1:AM376"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X85" sqref="X85"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16"/>
@@ -23671,7 +23668,7 @@
       <c r="X9" s="32">
         <v>0</v>
       </c>
-      <c r="Z9" s="136"/>
+      <c r="Z9" s="135"/>
     </row>
     <row r="10" spans="1:34">
       <c r="R10" s="22" t="s">
@@ -24066,16 +24063,16 @@
         <v>7</v>
       </c>
       <c r="T19" s="1"/>
-      <c r="U19" s="32" t="s">
+      <c r="U19" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="V19" s="32" t="s">
+      <c r="V19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="W19" s="32" t="s">
+      <c r="W19" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="X19" s="32">
+      <c r="X19" s="18">
         <v>0</v>
       </c>
       <c r="Z19" s="3"/>
@@ -24102,10 +24099,10 @@
       </c>
       <c r="Q20" s="14"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
-      <c r="X20" s="32"/>
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="18"/>
+      <c r="X20" s="18"/>
       <c r="Z20" s="3"/>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
@@ -24135,16 +24132,16 @@
       </c>
       <c r="R21" s="15"/>
       <c r="T21" s="1"/>
-      <c r="U21" s="47" t="s">
+      <c r="U21" s="137" t="s">
         <v>274</v>
       </c>
-      <c r="V21" s="94" t="s">
+      <c r="V21" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="W21" s="94" t="s">
+      <c r="W21" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="X21" s="94">
+      <c r="X21" s="25">
         <v>1</v>
       </c>
       <c r="Z21" s="3"/>
@@ -24680,16 +24677,16 @@
       <c r="Q43" s="29"/>
       <c r="R43" s="29"/>
       <c r="S43" s="16"/>
-      <c r="U43" s="32" t="s">
+      <c r="U43" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="V43" s="32" t="s">
+      <c r="V43" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="W43" s="32" t="s">
+      <c r="W43" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="X43" s="32">
+      <c r="X43" s="10">
         <v>0</v>
       </c>
     </row>
@@ -24699,10 +24696,10 @@
       <c r="Q44" s="29"/>
       <c r="R44" s="29"/>
       <c r="S44" s="16"/>
-      <c r="U44" s="32"/>
-      <c r="V44" s="32"/>
-      <c r="W44" s="32"/>
-      <c r="X44" s="32"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
+      <c r="W44" s="10"/>
+      <c r="X44" s="10"/>
       <c r="Z44" s="3" t="s">
         <v>162</v>
       </c>
@@ -24719,19 +24716,19 @@
       <c r="Q45" s="29"/>
       <c r="R45" s="29"/>
       <c r="S45" s="16"/>
-      <c r="U45" s="47" t="s">
+      <c r="U45" s="99" t="s">
         <v>274</v>
       </c>
-      <c r="V45" s="32" t="s">
+      <c r="V45" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="W45" s="138" t="s">
+      <c r="W45" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="X45" s="32">
+      <c r="X45" s="10">
         <v>1</v>
       </c>
-      <c r="Z45" s="137"/>
+      <c r="Z45" s="136"/>
     </row>
     <row r="46" spans="15:34">
       <c r="O46" s="16"/>
@@ -24739,10 +24736,10 @@
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="16"/>
-      <c r="U46" s="32"/>
-      <c r="V46" s="32"/>
-      <c r="W46" s="32"/>
-      <c r="X46" s="32"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="10"/>
+      <c r="W46" s="10"/>
+      <c r="X46" s="10"/>
       <c r="AD46" s="3" t="s">
         <v>159</v>
       </c>
@@ -24753,16 +24750,16 @@
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="16"/>
-      <c r="U47" s="92" t="s">
+      <c r="U47" s="33" t="s">
         <v>276</v>
       </c>
-      <c r="V47" s="94" t="s">
+      <c r="V47" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="W47" s="94" t="s">
+      <c r="W47" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="X47" s="94">
+      <c r="X47" s="24">
         <v>2</v>
       </c>
     </row>
@@ -24864,13 +24861,13 @@
       <c r="W52" s="32"/>
       <c r="X52" s="32"/>
       <c r="AB52" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="AF52" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="AG52" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="AF52" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="AG52" s="3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="53" spans="4:33">
@@ -24908,11 +24905,11 @@
       <c r="V54" s="32"/>
       <c r="W54" s="32"/>
       <c r="X54" s="32"/>
-      <c r="AA54" s="137" t="s">
+      <c r="AA54" s="136" t="s">
         <v>264</v>
       </c>
-      <c r="AB54" s="137"/>
-      <c r="AC54" s="137"/>
+      <c r="AB54" s="136"/>
+      <c r="AC54" s="136"/>
       <c r="AE54" s="72" t="s">
         <v>171</v>
       </c>
@@ -25281,7 +25278,7 @@
       <c r="AA70" s="1"/>
       <c r="AB70" s="2"/>
       <c r="AC70" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AD70" s="2"/>
       <c r="AF70" s="3" t="s">
@@ -25311,7 +25308,7 @@
         <v>83</v>
       </c>
       <c r="X71" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
@@ -25782,8 +25779,8 @@
       <c r="S84" s="29"/>
       <c r="U84" s="32"/>
       <c r="V84" s="32"/>
-      <c r="W84" s="95"/>
-      <c r="X84" s="95"/>
+      <c r="W84" s="94"/>
+      <c r="X84" s="94"/>
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
       <c r="AC84" s="1" t="s">
@@ -30384,7 +30381,7 @@
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
       <c r="M2" s="38"/>
-      <c r="Q2" s="116" t="s">
+      <c r="Q2" s="115" t="s">
         <v>69</v>
       </c>
       <c r="R2" s="39" t="s">
@@ -30392,7 +30389,7 @@
       </c>
     </row>
     <row r="3" spans="1:35">
-      <c r="Q3" s="117" t="s">
+      <c r="Q3" s="116" t="s">
         <v>70</v>
       </c>
       <c r="R3" s="39" t="s">
@@ -30400,7 +30397,7 @@
       </c>
     </row>
     <row r="4" spans="1:35">
-      <c r="Q4" s="116" t="s">
+      <c r="Q4" s="115" t="s">
         <v>82</v>
       </c>
       <c r="R4" s="39" t="s">
@@ -30408,7 +30405,7 @@
       </c>
     </row>
     <row r="5" spans="1:35">
-      <c r="Q5" s="117" t="s">
+      <c r="Q5" s="116" t="s">
         <v>83</v>
       </c>
       <c r="R5" s="39" t="s">
@@ -30422,7 +30419,7 @@
       <c r="R6" s="39"/>
     </row>
     <row r="7" spans="1:35">
-      <c r="Q7" s="104" t="s">
+      <c r="Q7" s="103" t="s">
         <v>80</v>
       </c>
       <c r="R7" s="39"/>
@@ -30450,12 +30447,12 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
-      <c r="N9" s="118" t="s">
+      <c r="N9" s="117" t="s">
         <v>106</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
-      <c r="Q9" s="119" t="s">
+      <c r="Q9" s="118" t="s">
         <v>79</v>
       </c>
     </row>
@@ -30470,14 +30467,14 @@
       <c r="J10" s="38"/>
       <c r="K10" s="38"/>
       <c r="L10" s="38"/>
-      <c r="N10" s="118" t="s">
+      <c r="N10" s="117" t="s">
         <v>105</v>
       </c>
       <c r="O10" s="15" t="s">
         <v>105</v>
       </c>
       <c r="P10" s="15"/>
-      <c r="Q10" s="119" t="s">
+      <c r="Q10" s="118" t="s">
         <v>80</v>
       </c>
       <c r="R10" s="39"/>
@@ -30486,14 +30483,14 @@
       <c r="M11" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="N11" s="118" t="s">
+      <c r="N11" s="117" t="s">
         <v>104</v>
       </c>
       <c r="O11" s="15" t="s">
         <v>104</v>
       </c>
       <c r="P11" s="15"/>
-      <c r="Q11" s="119" t="s">
+      <c r="Q11" s="118" t="s">
         <v>81</v>
       </c>
     </row>
@@ -30509,7 +30506,7 @@
         <v>92</v>
       </c>
       <c r="P12" s="15"/>
-      <c r="Q12" s="102" t="s">
+      <c r="Q12" s="101" t="s">
         <v>84</v>
       </c>
       <c r="R12" s="2"/>
@@ -30600,7 +30597,7 @@
     </row>
     <row r="16" spans="1:35">
       <c r="M16" s="55"/>
-      <c r="N16" s="120" t="s">
+      <c r="N16" s="119" t="s">
         <v>95</v>
       </c>
       <c r="Q16" s="10" t="s">
@@ -30627,13 +30624,13 @@
     </row>
     <row r="17" spans="1:39">
       <c r="I17" s="2"/>
-      <c r="J17" s="121" t="s">
+      <c r="J17" s="120" t="s">
         <v>94</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="55"/>
-      <c r="N17" s="122" t="s">
+      <c r="N17" s="121" t="s">
         <v>98</v>
       </c>
       <c r="O17" s="15" t="s">
@@ -30664,7 +30661,7 @@
     </row>
     <row r="18" spans="1:39">
       <c r="I18" s="2"/>
-      <c r="J18" s="121" t="s">
+      <c r="J18" s="120" t="s">
         <v>93</v>
       </c>
       <c r="K18" s="2" t="s">
@@ -30676,7 +30673,7 @@
       <c r="M18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N18" s="122" t="s">
+      <c r="N18" s="121" t="s">
         <v>101</v>
       </c>
       <c r="O18" s="15" t="s">
@@ -30709,7 +30706,7 @@
       <c r="I19" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="121" t="s">
+      <c r="J19" s="120" t="s">
         <v>92</v>
       </c>
       <c r="K19" s="8" t="s">
@@ -30836,7 +30833,7 @@
       <c r="P21" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="Q21" s="117" t="s">
+      <c r="Q21" s="116" t="s">
         <v>84</v>
       </c>
       <c r="R21" s="2"/>
@@ -30874,11 +30871,11 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="99"/>
+      <c r="M22" s="98"/>
       <c r="N22" s="16"/>
       <c r="O22" s="39"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="117" t="s">
+      <c r="Q22" s="116" t="s">
         <v>85</v>
       </c>
       <c r="R22" s="2"/>
@@ -30922,7 +30919,7 @@
       <c r="N23" s="16"/>
       <c r="O23" s="39"/>
       <c r="P23" s="2"/>
-      <c r="Q23" s="117" t="s">
+      <c r="Q23" s="116" t="s">
         <v>86</v>
       </c>
       <c r="R23" s="2"/>
@@ -30960,7 +30957,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="109" t="s">
+      <c r="M24" s="108" t="s">
         <v>92</v>
       </c>
       <c r="N24" s="15" t="s">
@@ -31003,7 +31000,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="109" t="s">
+      <c r="M25" s="108" t="s">
         <v>107</v>
       </c>
       <c r="N25" s="15" t="s">
@@ -31046,7 +31043,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="109">
+      <c r="M26" s="108">
         <v>2</v>
       </c>
       <c r="N26" s="15">
@@ -31131,7 +31128,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="14"/>
-      <c r="N28" s="123" t="s">
+      <c r="N28" s="122" t="s">
         <v>106</v>
       </c>
       <c r="O28" s="39"/>
@@ -31172,7 +31169,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="14"/>
-      <c r="N29" s="123" t="s">
+      <c r="N29" s="122" t="s">
         <v>105</v>
       </c>
       <c r="O29" s="15" t="s">
@@ -31217,7 +31214,7 @@
       <c r="M30" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="N30" s="123" t="s">
+      <c r="N30" s="122" t="s">
         <v>104</v>
       </c>
       <c r="O30" s="15" t="s">
@@ -31234,7 +31231,7 @@
       <c r="Z30" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="AA30" s="98" t="s">
+      <c r="AA30" s="97" t="s">
         <v>0</v>
       </c>
       <c r="AB30" s="2"/>
@@ -31322,7 +31319,7 @@
       <c r="V32" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="W32" s="98" t="s">
+      <c r="W32" s="97" t="s">
         <v>2</v>
       </c>
       <c r="X32" s="2"/>
@@ -31333,7 +31330,7 @@
       <c r="AC32" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AD32" s="98" t="s">
+      <c r="AD32" s="97" t="s">
         <v>2</v>
       </c>
       <c r="AE32" s="2"/>
@@ -31341,7 +31338,7 @@
       <c r="AG32" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="AH32" s="98" t="s">
+      <c r="AH32" s="97" t="s">
         <v>4</v>
       </c>
       <c r="AI32" s="2"/>
@@ -31417,38 +31414,38 @@
       <c r="T34" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="U34" s="98" t="s">
+      <c r="U34" s="97" t="s">
         <v>4</v>
       </c>
       <c r="V34" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="W34" s="98" t="s">
+      <c r="W34" s="97" t="s">
         <v>6</v>
       </c>
       <c r="X34" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="Y34" s="98" t="s">
+      <c r="Y34" s="97" t="s">
         <v>4</v>
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="AB34" s="98" t="s">
+      <c r="AB34" s="97" t="s">
         <v>4</v>
       </c>
       <c r="AC34" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="AD34" s="98" t="s">
+      <c r="AD34" s="97" t="s">
         <v>6</v>
       </c>
       <c r="AE34" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="AF34" s="98" t="s">
+      <c r="AF34" s="97" t="s">
         <v>4</v>
       </c>
       <c r="AG34" s="39"/>
@@ -31472,7 +31469,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="44"/>
-      <c r="N35" s="122" t="s">
+      <c r="N35" s="121" t="s">
         <v>95</v>
       </c>
       <c r="O35" s="39"/>
@@ -31520,14 +31517,14 @@
       <c r="F36" s="39"/>
       <c r="G36" s="39"/>
       <c r="H36" s="40"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="124" t="s">
+      <c r="I36" s="98"/>
+      <c r="J36" s="123" t="s">
         <v>96</v>
       </c>
       <c r="K36" s="39"/>
       <c r="L36" s="39"/>
       <c r="M36" s="44"/>
-      <c r="N36" s="122" t="s">
+      <c r="N36" s="121" t="s">
         <v>98</v>
       </c>
       <c r="O36" s="15" t="s">
@@ -31550,8 +31547,8 @@
       </c>
       <c r="G37" s="16"/>
       <c r="H37" s="39"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="124" t="s">
+      <c r="I37" s="98"/>
+      <c r="J37" s="123" t="s">
         <v>99</v>
       </c>
       <c r="K37" s="39" t="s">
@@ -31563,7 +31560,7 @@
       <c r="M37" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N37" s="122" t="s">
+      <c r="N37" s="121" t="s">
         <v>101</v>
       </c>
       <c r="O37" s="15" t="s">
@@ -31608,16 +31605,16 @@
       <c r="H38" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="I38" s="99" t="s">
+      <c r="I38" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="J38" s="124" t="s">
+      <c r="J38" s="123" t="s">
         <v>103</v>
       </c>
-      <c r="K38" s="100" t="s">
+      <c r="K38" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="L38" s="100" t="s">
+      <c r="L38" s="99" t="s">
         <v>103</v>
       </c>
       <c r="M38" s="48" t="s">
@@ -31720,10 +31717,10 @@
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
       <c r="D40" s="16"/>
-      <c r="E40" s="125">
+      <c r="E40" s="124">
         <v>0</v>
       </c>
-      <c r="F40" s="126">
+      <c r="F40" s="125">
         <v>0</v>
       </c>
       <c r="G40" s="20">
@@ -32041,7 +32038,7 @@
       <c r="A47" s="39"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
-      <c r="D47" s="127"/>
+      <c r="D47" s="126"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -32086,7 +32083,7 @@
     <row r="48" spans="1:39">
       <c r="A48" s="39"/>
       <c r="C48" s="39"/>
-      <c r="D48" s="127"/>
+      <c r="D48" s="126"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -32143,7 +32140,7 @@
       <c r="K49" s="16"/>
       <c r="L49" s="16"/>
       <c r="M49" s="2"/>
-      <c r="N49" s="118" t="s">
+      <c r="N49" s="117" t="s">
         <v>106</v>
       </c>
       <c r="O49" s="2"/>
@@ -32184,7 +32181,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
-      <c r="N50" s="118" t="s">
+      <c r="N50" s="117" t="s">
         <v>105</v>
       </c>
       <c r="O50" s="15" t="s">
@@ -32229,7 +32226,7 @@
       <c r="M51" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="N51" s="118" t="s">
+      <c r="N51" s="117" t="s">
         <v>104</v>
       </c>
       <c r="O51" s="15" t="s">
@@ -32440,7 +32437,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
       <c r="M56" s="55"/>
-      <c r="N56" s="120" t="s">
+      <c r="N56" s="119" t="s">
         <v>95</v>
       </c>
       <c r="O56" s="2"/>
@@ -32475,13 +32472,13 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="J57" s="121" t="s">
+      <c r="J57" s="120" t="s">
         <v>94</v>
       </c>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
       <c r="M57" s="44"/>
-      <c r="N57" s="120" t="s">
+      <c r="N57" s="119" t="s">
         <v>98</v>
       </c>
       <c r="O57" s="15" t="s">
@@ -32518,7 +32515,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="121" t="s">
+      <c r="J58" s="120" t="s">
         <v>93</v>
       </c>
       <c r="K58" s="2" t="s">
@@ -32530,7 +32527,7 @@
       <c r="M58" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="N58" s="120" t="s">
+      <c r="N58" s="119" t="s">
         <v>101</v>
       </c>
       <c r="O58" s="15" t="s">
@@ -32569,7 +32566,7 @@
       <c r="I59" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="J59" s="128" t="s">
+      <c r="J59" s="127" t="s">
         <v>92</v>
       </c>
       <c r="K59" s="20" t="s">
@@ -32617,7 +32614,7 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-      <c r="I60" s="129" t="s">
+      <c r="I60" s="128" t="s">
         <v>102</v>
       </c>
       <c r="J60" s="83" t="s">
@@ -32667,7 +32664,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
-      <c r="I61" s="129">
+      <c r="I61" s="128">
         <v>1</v>
       </c>
       <c r="J61" s="83">
@@ -33000,7 +32997,7 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="N69" s="118" t="s">
+      <c r="N69" s="117" t="s">
         <v>106</v>
       </c>
       <c r="O69" s="2"/>
@@ -33046,7 +33043,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="N70" s="118" t="s">
+      <c r="N70" s="117" t="s">
         <v>105</v>
       </c>
       <c r="O70" s="15" t="s">
@@ -33097,7 +33094,7 @@
       <c r="M71" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="N71" s="118" t="s">
+      <c r="N71" s="117" t="s">
         <v>104</v>
       </c>
       <c r="O71" s="15" t="s">
@@ -33148,10 +33145,10 @@
       <c r="M72" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N72" s="117" t="s">
+      <c r="N72" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="O72" s="130" t="s">
+      <c r="O72" s="129" t="s">
         <v>103</v>
       </c>
       <c r="P72" s="15"/>
@@ -33199,10 +33196,10 @@
       <c r="M73" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="N73" s="117" t="s">
+      <c r="N73" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="O73" s="130" t="s">
+      <c r="O73" s="129" t="s">
         <v>102</v>
       </c>
       <c r="P73" s="15"/>
@@ -33250,10 +33247,10 @@
       <c r="M74" s="12">
         <v>2</v>
       </c>
-      <c r="N74" s="117">
+      <c r="N74" s="116">
         <v>2</v>
       </c>
-      <c r="O74" s="130">
+      <c r="O74" s="129">
         <v>3</v>
       </c>
       <c r="P74" s="15" t="s">
@@ -33342,7 +33339,7 @@
       <c r="K76" s="39"/>
       <c r="L76" s="39"/>
       <c r="M76" s="55"/>
-      <c r="N76" s="120" t="s">
+      <c r="N76" s="119" t="s">
         <v>95</v>
       </c>
       <c r="O76" s="2"/>
@@ -33375,14 +33372,14 @@
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
-      <c r="I77" s="99"/>
-      <c r="J77" s="131" t="s">
+      <c r="I77" s="98"/>
+      <c r="J77" s="130" t="s">
         <v>96</v>
       </c>
       <c r="K77" s="16"/>
       <c r="L77" s="16"/>
       <c r="M77" s="13"/>
-      <c r="N77" s="120" t="s">
+      <c r="N77" s="119" t="s">
         <v>98</v>
       </c>
       <c r="O77" s="15" t="s">
@@ -33413,15 +33410,15 @@
       <c r="AM77" s="2"/>
     </row>
     <row r="78" spans="1:44">
-      <c r="D78" s="127"/>
+      <c r="D78" s="126"/>
       <c r="E78" s="16"/>
       <c r="F78" s="16" t="s">
         <v>97</v>
       </c>
       <c r="G78" s="16"/>
       <c r="H78" s="16"/>
-      <c r="I78" s="99"/>
-      <c r="J78" s="132" t="s">
+      <c r="I78" s="98"/>
+      <c r="J78" s="131" t="s">
         <v>99</v>
       </c>
       <c r="K78" s="16" t="s">
@@ -33433,7 +33430,7 @@
       <c r="M78" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="N78" s="120" t="s">
+      <c r="N78" s="119" t="s">
         <v>101</v>
       </c>
       <c r="O78" s="15" t="s">
@@ -33460,7 +33457,7 @@
       <c r="AJ78" s="2"/>
     </row>
     <row r="79" spans="1:44">
-      <c r="D79" s="127"/>
+      <c r="D79" s="126"/>
       <c r="E79" s="16"/>
       <c r="F79" s="16" t="s">
         <v>100</v>
@@ -33471,22 +33468,22 @@
       <c r="H79" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="I79" s="99" t="s">
+      <c r="I79" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="J79" s="132" t="s">
+      <c r="J79" s="131" t="s">
         <v>103</v>
       </c>
-      <c r="K79" s="126" t="s">
+      <c r="K79" s="125" t="s">
         <v>103</v>
       </c>
-      <c r="L79" s="116" t="s">
+      <c r="L79" s="115" t="s">
         <v>103</v>
       </c>
       <c r="M79" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="N79" s="117" t="s">
+      <c r="N79" s="116" t="s">
         <v>103</v>
       </c>
       <c r="O79" s="15" t="s">
@@ -33513,7 +33510,7 @@
       <c r="AJ79" s="2"/>
     </row>
     <row r="80" spans="1:44">
-      <c r="D80" s="127" t="s">
+      <c r="D80" s="126" t="s">
         <v>69</v>
       </c>
       <c r="E80" s="16" t="s">
@@ -33528,22 +33525,22 @@
       <c r="H80" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="I80" s="111" t="s">
+      <c r="I80" s="110" t="s">
         <v>102</v>
       </c>
       <c r="J80" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="K80" s="126" t="s">
+      <c r="K80" s="125" t="s">
         <v>102</v>
       </c>
-      <c r="L80" s="126" t="s">
+      <c r="L80" s="125" t="s">
         <v>102</v>
       </c>
       <c r="M80" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="N80" s="117" t="s">
+      <c r="N80" s="116" t="s">
         <v>102</v>
       </c>
       <c r="O80" s="15" t="s">
@@ -33570,13 +33567,13 @@
       <c r="AJ80" s="2"/>
     </row>
     <row r="81" spans="4:36">
-      <c r="D81" s="133">
+      <c r="D81" s="132">
         <v>0</v>
       </c>
-      <c r="E81" s="126">
+      <c r="E81" s="125">
         <v>0</v>
       </c>
-      <c r="F81" s="126">
+      <c r="F81" s="125">
         <v>0</v>
       </c>
       <c r="G81" s="83">
@@ -33585,22 +33582,22 @@
       <c r="H81" s="83">
         <v>1</v>
       </c>
-      <c r="I81" s="111">
+      <c r="I81" s="110">
         <v>1</v>
       </c>
       <c r="J81" s="83">
         <v>1</v>
       </c>
-      <c r="K81" s="126">
+      <c r="K81" s="125">
         <v>2</v>
       </c>
-      <c r="L81" s="126">
+      <c r="L81" s="125">
         <v>2</v>
       </c>
       <c r="M81" s="12">
         <v>2</v>
       </c>
-      <c r="N81" s="117">
+      <c r="N81" s="116">
         <v>2</v>
       </c>
       <c r="O81" s="15">
@@ -33629,7 +33626,7 @@
       <c r="AJ81" s="2"/>
     </row>
     <row r="82" spans="4:36">
-      <c r="D82" s="127"/>
+      <c r="D82" s="126"/>
       <c r="E82" s="16"/>
       <c r="F82" s="16"/>
       <c r="G82" s="16"/>
@@ -33660,7 +33657,7 @@
       <c r="AJ82" s="2"/>
     </row>
     <row r="83" spans="4:36" s="2" customFormat="1">
-      <c r="D83" s="127"/>
+      <c r="D83" s="126"/>
       <c r="E83" s="16"/>
       <c r="F83" s="39"/>
       <c r="G83" s="39"/>
@@ -33671,7 +33668,7 @@
       </c>
     </row>
     <row r="84" spans="4:36" s="2" customFormat="1">
-      <c r="D84" s="127"/>
+      <c r="D84" s="126"/>
       <c r="E84" s="16"/>
       <c r="F84" s="39"/>
       <c r="G84" s="39"/>
@@ -33686,7 +33683,7 @@
       <c r="O84" s="15"/>
     </row>
     <row r="85" spans="4:36" s="2" customFormat="1">
-      <c r="D85" s="127"/>
+      <c r="D85" s="126"/>
       <c r="I85" s="13"/>
       <c r="M85" s="12" t="s">
         <v>102</v>
@@ -33697,7 +33694,7 @@
       <c r="O85" s="15"/>
     </row>
     <row r="86" spans="4:36" s="2" customFormat="1">
-      <c r="D86" s="127"/>
+      <c r="D86" s="126"/>
       <c r="I86" s="13"/>
       <c r="M86" s="12">
         <v>2</v>
@@ -33710,7 +33707,7 @@
       </c>
     </row>
     <row r="87" spans="4:36" s="2" customFormat="1">
-      <c r="D87" s="127"/>
+      <c r="D87" s="126"/>
       <c r="E87" s="16"/>
       <c r="F87" s="39"/>
       <c r="G87" s="39"/>
@@ -33739,7 +33736,7 @@
       </c>
       <c r="G88" s="39"/>
       <c r="H88" s="39"/>
-      <c r="I88" s="111" t="s">
+      <c r="I88" s="110" t="s">
         <v>102</v>
       </c>
       <c r="J88" s="2" t="s">
@@ -33760,7 +33757,7 @@
       <c r="Y88" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="Z88" s="106" t="s">
+      <c r="Z88" s="105" t="s">
         <v>81</v>
       </c>
       <c r="AA88" s="14"/>
@@ -33768,7 +33765,7 @@
       <c r="AC88" s="14"/>
     </row>
     <row r="89" spans="4:36">
-      <c r="E89" s="125">
+      <c r="E89" s="124">
         <v>0</v>
       </c>
       <c r="F89" s="15">
@@ -33778,7 +33775,7 @@
         <v>73</v>
       </c>
       <c r="H89" s="39"/>
-      <c r="I89" s="111">
+      <c r="I89" s="110">
         <v>1</v>
       </c>
       <c r="J89" s="2">
@@ -33793,10 +33790,10 @@
       <c r="T89" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="U89" s="134" t="s">
+      <c r="U89" s="133" t="s">
         <v>69</v>
       </c>
-      <c r="V89" s="106" t="s">
+      <c r="V89" s="105" t="s">
         <v>82</v>
       </c>
       <c r="W89" s="14" t="s">
@@ -33808,7 +33805,7 @@
       <c r="Y89" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="Z89" s="106" t="s">
+      <c r="Z89" s="105" t="s">
         <v>102</v>
       </c>
       <c r="AA89" s="14" t="s">
@@ -33823,10 +33820,10 @@
       <c r="T90" s="14">
         <v>0</v>
       </c>
-      <c r="U90" s="134">
+      <c r="U90" s="133">
         <v>0</v>
       </c>
-      <c r="V90" s="106">
+      <c r="V90" s="105">
         <v>0</v>
       </c>
       <c r="W90" s="14">
@@ -33838,7 +33835,7 @@
       <c r="Y90" s="14">
         <v>1</v>
       </c>
-      <c r="Z90" s="106">
+      <c r="Z90" s="105">
         <v>1</v>
       </c>
       <c r="AA90" s="14">
@@ -33852,12 +33849,12 @@
       </c>
     </row>
     <row r="91" spans="4:36">
-      <c r="U91" s="135"/>
+      <c r="U91" s="134"/>
       <c r="V91" s="55"/>
       <c r="Z91" s="55"/>
     </row>
     <row r="92" spans="4:36">
-      <c r="U92" s="135" t="s">
+      <c r="U92" s="134" t="s">
         <v>69</v>
       </c>
       <c r="V92" s="55" t="s">
@@ -33899,7 +33896,7 @@
       </c>
     </row>
     <row r="2" spans="1:30">
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="96" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -33913,7 +33910,7 @@
       <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="96" t="s">
         <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -33921,7 +33918,7 @@
       </c>
     </row>
     <row r="4" spans="1:30">
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="96" t="s">
         <v>36</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -33953,7 +33950,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="H6" s="97"/>
+      <c r="H6" s="96"/>
     </row>
     <row r="7" spans="1:30">
       <c r="C7" s="4"/>
@@ -33963,16 +33960,16 @@
       <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="97"/>
+      <c r="H7" s="96"/>
     </row>
     <row r="8" spans="1:30">
       <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="97"/>
+      <c r="H8" s="96"/>
     </row>
     <row r="9" spans="1:30">
-      <c r="H9" s="97"/>
+      <c r="H9" s="96"/>
     </row>
     <row r="11" spans="1:30">
       <c r="B11" s="1" t="s">

</xml_diff>